<commit_message>
docs: add class diagarm for sprint01
</commit_message>
<xml_diff>
--- a/doc/Sprint01/routes table/routes_table.xlsx
+++ b/doc/Sprint01/routes table/routes_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrirahmanto/flask/fishapi/doc/Sprint01/routes table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C790898-0A12-8C47-B955-0DDDC7AFA516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE8566E-1502-BC49-A6D1-F00B881BC6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16000" xr2:uid="{C254AC1B-B4CF-49CB-B06F-3FDC00B6733D}"/>
   </bookViews>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9212EE-4B8C-4B45-BD8A-30CF3A593525}">
   <dimension ref="A2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>